<commit_message>
Specs edit and Project management
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cole\Documents\Fall 2018\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E5A38C-65CF-4A8F-941F-29B349431B7C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97269D4-B2DF-4BBF-9A21-30E5AF2BA50E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4170" xr2:uid="{CAACB808-7CD7-4C72-AD89-1ECCC547C117}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>9 days</t>
+  </si>
+  <si>
+    <t>Deliver Preliminary design presentation</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -188,6 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C52C06E-316C-4A3E-83A4-1B8BF9A40FF6}">
-  <dimension ref="A1:BG20"/>
+  <dimension ref="A1:BG21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,18 +818,18 @@
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="6"/>
-      <c r="AE7" s="6"/>
-      <c r="AF7" s="6"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -906,47 +910,54 @@
       <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="M15" s="6"/>
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="E16" s="2"/>
+      <c r="N16" s="6"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="O16" s="6"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>26</v>
-      </c>
       <c r="E17" s="2"/>
-      <c r="R17" s="6"/>
+      <c r="O17" s="6"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2"/>
       <c r="R18" s="6"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
+      <c r="R19" s="6"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="T20" s="6"/>
+      <c r="E21" s="2"/>
+      <c r="T21" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>